<commit_message>
Finalised tests + implementation
</commit_message>
<xml_diff>
--- a/Assignment  - REST API Design.xlsx
+++ b/Assignment  - REST API Design.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Desktop\Third Year Material\CO3409 Enterprise Application Development\Assignment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AC629E0-2EEC-4DA2-AF7A-97C70B9FCCA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{032B6CBA-C301-4065-BA1C-0C7034FE9BD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="47">
   <si>
     <t>No.</t>
   </si>
@@ -235,9 +235,6 @@
 ]</t>
   </si>
   <si>
-    <t>api/initialise</t>
-  </si>
-  <si>
     <t>[
   {
     links: { href: "/questions/{username}"}
@@ -314,6 +311,26 @@
     links: { href: "/initialise"}
   }
 ]</t>
+  </si>
+  <si>
+    <t>api/question/{username}/submit/picture</t>
+  </si>
+  <si>
+    <t>400, 404, 415, 422</t>
+  </si>
+  <si>
+    <t>User submits their answer as a picture. They would attach a picture to the request in the body as form-data A.K.A multipart/form-data.</t>
+  </si>
+  <si>
+    <t>form-data
+[
+    {
+        picture: &lt;upload picture&gt;
+    }
+]</t>
+  </si>
+  <si>
+    <t>api/categories</t>
   </si>
 </sst>
 </file>
@@ -704,8 +721,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -715,7 +732,7 @@
     <col min="3" max="3" width="44.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="38.85546875" customWidth="1"/>
     <col min="5" max="5" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="51.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="26.7109375" bestFit="1" customWidth="1"/>
   </cols>
@@ -754,7 +771,7 @@
         <v>7</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>8</v>
@@ -766,7 +783,7 @@
         <v>21</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H2" s="1"/>
     </row>
@@ -790,7 +807,7 @@
         <v>21</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>34</v>
@@ -827,51 +844,51 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>20</v>
+        <v>45</v>
       </c>
       <c r="E5" s="1">
         <v>200</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>22</v>
+        <v>43</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="E6" s="1">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>22</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>8</v>
+        <v>38</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="90" x14ac:dyDescent="0.25">
@@ -879,25 +896,25 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>8</v>
+        <v>31</v>
       </c>
       <c r="E7" s="1">
-        <v>200</v>
+        <v>204</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>22</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="90" x14ac:dyDescent="0.25">
@@ -908,7 +925,7 @@
         <v>7</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>8</v>
@@ -926,17 +943,17 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="210" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D9" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E9" s="1">
@@ -946,21 +963,21 @@
         <v>22</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="210" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>8</v>
@@ -972,13 +989,13 @@
         <v>22</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>18</v>
+        <v>39</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="240" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -986,7 +1003,7 @@
         <v>7</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>8</v>
@@ -995,26 +1012,40 @@
         <v>200</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="240" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>11</v>
       </c>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
+      <c r="B12" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12" s="1">
+        <v>200</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1">

</xml_diff>